<commit_message>
phrasing of output text changes (#4)
</commit_message>
<xml_diff>
--- a/external_data_test/office_hours.xlsx
+++ b/external_data_test/office_hours.xlsx
@@ -35,9 +35,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -111,7 +112,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -125,6 +126,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,10 +210,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -229,14 +234,44 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
+        <v>45063</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>45402</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B4" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C4" s="1" t="n">
         <v>18</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>